<commit_message>
78: Fixed one ASC issue. Named V0.33. (Date20250523)
</commit_message>
<xml_diff>
--- a/Objects/PGS7-0-32_20250523-BurnFile/PGS7_FW_ChangeNote.xlsx
+++ b/Objects/PGS7-0-32_20250523-BurnFile/PGS7_FW_ChangeNote.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20917" windowHeight="9060"/>
+    <workbookView windowWidth="20917" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="PGS7" sheetId="1" r:id="rId1"/>
@@ -1302,7 +1302,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>

</xml_diff>